<commit_message>
new examples using UCC
</commit_message>
<xml_diff>
--- a/C_35allEdited.xlsx
+++ b/C_35allEdited.xlsx
@@ -5,21 +5,29 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ijohnson/wErika/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ijohnson/Documents/GitHub/ColoredCubePuzzle/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{44258B85-AA13-4849-82C8-176A8DE44AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6305EFB-B08D-AE41-A3BC-5E4691A35CCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5560" yWindow="-20580" windowWidth="24620" windowHeight="16660" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="140" yWindow="940" windowWidth="24620" windowHeight="16660" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="C_35all" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -119,7 +127,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
+  <dxfs count="8">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -197,286 +205,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC0FFEE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0070C0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFC000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEECBFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFC000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEECBFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEECBFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -765,7 +493,7 @@
   <dimension ref="A1:J76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>